<commit_message>
Uploaded doorlift door brackets
</commit_message>
<xml_diff>
--- a/Part File Library/Printed parts list.xlsx
+++ b/Part File Library/Printed parts list.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Part File Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="563" documentId="8_{BD805E17-6825-4CEB-B659-8E3FDADE9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{620A7BD0-74FD-42AB-9AB0-2F779F920224}"/>
+  <xr:revisionPtr revIDLastSave="580" documentId="8_{BD805E17-6825-4CEB-B659-8E3FDADE9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F583C1F-DA92-4612-BFA0-7B61AF21D6F7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F5C623C1-69F2-4E87-8B60-6F2BB08936E1}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{F5C623C1-69F2-4E87-8B60-6F2BB08936E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$H$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$H$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="88">
   <si>
     <t>System</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>add your price</t>
+  </si>
+  <si>
+    <t>Doorlift Door Bracket A_1x</t>
+  </si>
+  <si>
+    <t>Doorlift Door Bracket B_1x</t>
   </si>
 </sst>
 </file>
@@ -778,7 +784,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5107985C-7B0C-435D-8112-62AC3AA4572D}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -810,12 +816,12 @@
       <c r="D1" s="8"/>
       <c r="E1" s="6"/>
       <c r="F1" s="9">
-        <f>F65</f>
-        <v>4.4652777777777759</v>
+        <f>F67</f>
+        <v>4.6319444444444429</v>
       </c>
       <c r="G1" s="11">
-        <f>G65</f>
-        <v>3057</v>
+        <f>G67</f>
+        <v>3217</v>
       </c>
       <c r="H1" s="10"/>
     </row>
@@ -845,7 +851,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="21">
         <f>G1*B3</f>
-        <v>122.28</v>
+        <v>128.68</v>
       </c>
       <c r="H3" s="15"/>
     </row>
@@ -896,7 +902,7 @@
         <v>2.5694444444444447E-2</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G45" si="1">E5*D5</f>
+        <f t="shared" ref="G5:G47" si="1">E5*D5</f>
         <v>22</v>
       </c>
       <c r="H5" t="s">
@@ -1068,7 +1074,7 @@
         <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1788,7 +1794,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" ref="F37:F63" si="3">E37*C37</f>
+        <f t="shared" ref="F37:F65" si="3">E37*C37</f>
         <v>4.7222222222222221E-2</v>
       </c>
       <c r="G37" s="3">
@@ -1888,24 +1894,24 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="C41" s="2">
-        <v>1.1111111111111112E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D41" s="4">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="3"/>
-        <v>2.2222222222222223E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G41" s="3">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="H41" t="s">
         <v>15</v>
@@ -1916,24 +1922,24 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2">
-        <v>3.125E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D42" s="4">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="3"/>
-        <v>3.125E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G42" s="3">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="H42" t="s">
         <v>15</v>
@@ -1944,24 +1950,24 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C43" s="2">
-        <v>3.125E-2</v>
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="D43" s="4">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="3"/>
-        <v>3.125E-2</v>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="G43" s="3">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H43" t="s">
         <v>15</v>
@@ -1972,27 +1978,27 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C44" s="2">
-        <v>1.3194444444444444E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="D44" s="4">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E44">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="3"/>
-        <v>5.2777777777777778E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="G44" s="3">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="H44" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2000,27 +2006,27 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C45" s="2">
-        <v>1.5277777777777777E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="D45" s="4">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="3"/>
-        <v>3.0555555555555555E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="G45" s="3">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H45" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2028,27 +2034,27 @@
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C46" s="2">
-        <v>0.41666666666666669</v>
+        <v>1.3194444444444444E-2</v>
       </c>
       <c r="D46" s="4">
-        <v>400</v>
+        <v>11</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="3"/>
-        <v>0.41666666666666669</v>
+        <v>5.2777777777777778E-2</v>
       </c>
       <c r="G46" s="3">
-        <f>E46*D46</f>
-        <v>400</v>
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="H46" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2056,24 +2062,24 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C47" s="2">
-        <v>2.2916666666666669E-2</v>
+        <v>1.5277777777777777E-2</v>
       </c>
       <c r="D47" s="4">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="3"/>
-        <v>2.2916666666666669E-2</v>
+        <v>3.0555555555555555E-2</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" ref="G47:G63" si="4">E47*D47</f>
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
       <c r="H47" t="s">
         <v>73</v>
@@ -2084,83 +2090,83 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C48" s="2">
-        <v>2.2916666666666669E-2</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D48" s="4">
-        <v>19</v>
+        <v>400</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="3"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G48" s="3">
+        <f>E48*D48</f>
+        <v>400</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="2">
         <v>2.2916666666666669E-2</v>
       </c>
-      <c r="G48" s="3">
+      <c r="D49" s="4">
+        <v>19</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="G49" s="3">
+        <f t="shared" ref="G49:G65" si="4">E49*D49</f>
+        <v>19</v>
+      </c>
+      <c r="H49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="D50" s="4">
+        <v>19</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="G50" s="3">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H50" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="2">
-        <v>6.2499999999999995E-3</v>
-      </c>
-      <c r="D49" s="4">
-        <v>5</v>
-      </c>
-      <c r="E49">
-        <v>4</v>
-      </c>
-      <c r="F49" s="1">
-        <f t="shared" si="3"/>
-        <v>2.4999999999999998E-2</v>
-      </c>
-      <c r="G49" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="H49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B50" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="2">
-        <v>6.2499999999999995E-3</v>
-      </c>
-      <c r="D50" s="4">
-        <v>5</v>
-      </c>
-      <c r="E50">
-        <v>4</v>
-      </c>
-      <c r="F50" s="1">
-        <f t="shared" si="3"/>
-        <v>2.4999999999999998E-2</v>
-      </c>
-      <c r="G50" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="H50" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2168,24 +2174,24 @@
         <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C51" s="2">
-        <v>1.5277777777777777E-2</v>
+        <v>6.2499999999999995E-3</v>
       </c>
       <c r="D51" s="4">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="3"/>
-        <v>3.0555555555555555E-2</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="G51" s="3">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H51" t="s">
         <v>15</v>
@@ -2196,24 +2202,24 @@
         <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C52" s="2">
-        <v>0.16666666666666666</v>
+        <v>6.2499999999999995E-3</v>
       </c>
       <c r="D52" s="4">
-        <v>175</v>
+        <v>5</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="3"/>
-        <v>0.16666666666666666</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="G52" s="3">
         <f t="shared" si="4"/>
-        <v>175</v>
+        <v>20</v>
       </c>
       <c r="H52" t="s">
         <v>15</v>
@@ -2224,24 +2230,24 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C53" s="2">
-        <v>1.3888888888888888E-2</v>
+        <v>1.5277777777777777E-2</v>
       </c>
       <c r="D53" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E53">
         <v>2</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="3"/>
-        <v>2.7777777777777776E-2</v>
+        <v>3.0555555555555555E-2</v>
       </c>
       <c r="G53" s="3">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H53" t="s">
         <v>15</v>
@@ -2252,24 +2258,24 @@
         <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C54" s="2">
-        <v>0.19791666666666666</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D54" s="4">
-        <v>111</v>
+        <v>175</v>
       </c>
       <c r="E54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="3"/>
-        <v>0.39583333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G54" s="3">
         <f t="shared" si="4"/>
-        <v>222</v>
+        <v>175</v>
       </c>
       <c r="H54" t="s">
         <v>15</v>
@@ -2280,24 +2286,24 @@
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C55" s="2">
-        <v>2.7777777777777779E-3</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="D55" s="4">
+        <v>14</v>
+      </c>
+      <c r="E55">
         <v>2</v>
-      </c>
-      <c r="E55">
-        <v>3</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="3"/>
-        <v>8.3333333333333332E-3</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="G55" s="3">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="H55" t="s">
         <v>15</v>
@@ -2308,24 +2314,24 @@
         <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C56" s="2">
-        <v>8.5416666666666655E-2</v>
+        <v>0.19791666666666666</v>
       </c>
       <c r="D56" s="4">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="3"/>
-        <v>8.5416666666666655E-2</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="G56" s="3">
         <f t="shared" si="4"/>
-        <v>84</v>
+        <v>222</v>
       </c>
       <c r="H56" t="s">
         <v>15</v>
@@ -2336,24 +2342,24 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C57" s="2">
-        <v>3.3333333333333333E-2</v>
+        <v>2.7777777777777779E-3</v>
       </c>
       <c r="D57" s="4">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="G57" s="3">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="H57" t="s">
         <v>15</v>
@@ -2364,24 +2370,24 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C58" s="2">
-        <v>2.7777777777777776E-2</v>
+        <v>8.5416666666666655E-2</v>
       </c>
       <c r="D58" s="4">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="3"/>
-        <v>2.7777777777777776E-2</v>
+        <v>8.5416666666666655E-2</v>
       </c>
       <c r="G58" s="3">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="H58" t="s">
         <v>15</v>
@@ -2392,24 +2398,24 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C59" s="2">
-        <v>5.5555555555555558E-3</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="D59" s="4">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="3"/>
-        <v>5.5555555555555558E-3</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="G59" s="3">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="H59" t="s">
         <v>15</v>
@@ -2420,24 +2426,24 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C60" s="2">
-        <v>0.1076388888888889</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="D60" s="4">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="3"/>
-        <v>0.1076388888888889</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="G60" s="3">
         <f t="shared" si="4"/>
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="H60" t="s">
         <v>15</v>
@@ -2448,24 +2454,24 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C61" s="2">
-        <v>3.472222222222222E-3</v>
+        <v>5.5555555555555558E-3</v>
       </c>
       <c r="D61" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="3"/>
-        <v>1.0416666666666666E-2</v>
+        <v>5.5555555555555558E-3</v>
       </c>
       <c r="G61" s="3">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H61" t="s">
         <v>15</v>
@@ -2476,24 +2482,24 @@
         <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C62" s="2">
-        <v>1.3888888888888889E-3</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="D62" s="4">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="1">
         <f t="shared" si="3"/>
-        <v>1.3888888888888889E-3</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="G62" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="H62" t="s">
         <v>15</v>
@@ -2504,82 +2510,138 @@
         <v>59</v>
       </c>
       <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D63" s="4">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G63" s="3">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="D64" s="4">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2">
+        <f t="shared" si="3"/>
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="G64" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C65" s="2">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D63" s="4">
-        <v>15</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63" s="2">
+      <c r="D65" s="4">
+        <v>15</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2">
         <f t="shared" si="3"/>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G65" s="3">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="H63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B67" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="9">
-        <f>SUM(F5:F63)</f>
-        <v>4.4652777777777759</v>
-      </c>
-      <c r="G65" s="11">
-        <f>SUM(G5:G64)</f>
-        <v>3057</v>
-      </c>
-      <c r="H65" s="10"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+      <c r="C67" s="7"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="9">
+        <f>SUM(F5:F65)</f>
+        <v>4.6319444444444429</v>
+      </c>
+      <c r="G67" s="11">
+        <f>SUM(G5:G66)</f>
+        <v>3217</v>
+      </c>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="H66" s="17"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="H68" s="17"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B67" s="18">
+      <c r="B69" s="18">
         <v>40</v>
       </c>
-      <c r="H67" s="17"/>
-    </row>
-    <row r="68" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="12" t="s">
+      <c r="H69" s="17"/>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B68" s="19">
-        <f>B67/1000</f>
+      <c r="B70" s="19">
+        <f>B69/1000</f>
         <v>0.04</v>
       </c>
-      <c r="C68" s="20"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="21">
-        <f>G65*B68</f>
-        <v>122.28</v>
-      </c>
-      <c r="H68" s="15"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="21">
+        <f>G67*B70</f>
+        <v>128.68</v>
+      </c>
+      <c r="H70" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>